<commit_message>
new draft with rewritten stylized facts. FIRE moved before stylized fact.
</commit_message>
<xml_diff>
--- a/workingfolder/python/tables/data_moments.xlsx
+++ b/workingfolder/python/tables/data_moments.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>SPF</t>
   </si>
@@ -28,6 +28,9 @@
     <t>FIRE+SV</t>
   </si>
   <si>
+    <t>SE+AR</t>
+  </si>
+  <si>
     <t>InfAV</t>
   </si>
   <si>
@@ -80,6 +83,12 @@
   </si>
   <si>
     <t>&gt;0</t>
+  </si>
+  <si>
+    <t>$\lambda^2\sigma^2/(1-(1-\lambda)^2\rho^2)$</t>
+  </si>
+  <si>
+    <t>$(1-\lambda)\rho\text{FEVar}$</t>
   </si>
 </sst>
 </file>
@@ -437,13 +446,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -456,10 +465,13 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>-0</v>
@@ -471,12 +483,15 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>20</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>1.145</v>
@@ -485,15 +500,18 @@
         <v>3.959</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>0.115</v>
@@ -502,15 +520,18 @@
         <v>0.417</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>-0.15</v>
@@ -524,10 +545,13 @@
       <c r="E5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>1.032</v>
@@ -536,15 +560,18 @@
         <v>3.794</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>21</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>0.006</v>
@@ -558,10 +585,13 @@
       <c r="E7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>0.2</v>
@@ -575,10 +605,13 @@
       <c r="E8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>0.042</v>
@@ -592,10 +625,13 @@
       <c r="E9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10">
         <v>0.01</v>
@@ -609,10 +645,13 @@
       <c r="E10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>0.246</v>
@@ -621,15 +660,18 @@
         <v>1.738</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>21</v>
+      </c>
+      <c r="F11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B12">
         <v>0.002</v>
@@ -641,12 +683,15 @@
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>22</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B13">
         <v>0.001</v>
@@ -658,7 +703,10 @@
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>